<commit_message>
Create and test Login page
</commit_message>
<xml_diff>
--- a/CURA_TCs.xlsx
+++ b/CURA_TCs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\robotframework_selenium_exercise\Projects\CURA_Healthcare_Service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visans49\Desktop\BOSS_GIT\CURA\web-cura-robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B7EF99-BE14-44FB-A6AE-CE81AEECC82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95565C0E-2F59-4372-81E5-EBC5C85BC927}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Confirmation" sheetId="5" r:id="rId4"/>
     <sheet name="Histories" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="192">
   <si>
     <t>Project Name:</t>
   </si>
@@ -179,7 +178,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -189,7 +188,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -199,7 +198,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -209,7 +208,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -224,7 +223,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -234,7 +233,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -244,7 +243,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -254,7 +253,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -269,7 +268,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -279,7 +278,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -289,7 +288,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -299,7 +298,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -314,7 +313,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -324,7 +323,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -334,7 +333,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -344,7 +343,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -388,7 +387,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -398,7 +397,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -409,7 +408,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -419,7 +418,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -434,7 +433,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -444,7 +443,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -455,7 +454,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -465,7 +464,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -666,7 +665,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -676,7 +675,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -713,7 +712,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -723,7 +722,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -742,7 +741,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -752,7 +751,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -771,7 +770,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -781,7 +780,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -800,7 +799,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -810,7 +809,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Tahoma"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1055,12 +1054,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1068,14 +1067,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1083,20 +1082,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1219,7 +1218,6 @@
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1271,7 +1269,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1302,7 +1299,6 @@
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1354,7 +1350,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1385,7 +1380,6 @@
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1437,7 +1431,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1468,7 +1461,6 @@
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1520,7 +1512,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1551,7 +1542,6 @@
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1603,7 +1593,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1628,110 +1617,110 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6AAF7161-9A61-4868-8257-1E638CA674CE}" name="Table13" displayName="Table13" ref="A8:M14" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
-  <autoFilter ref="A8:M14" xr:uid="{6AAF7161-9A61-4868-8257-1E638CA674CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:M14" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+  <autoFilter ref="A8:M14"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A433FD94-98B1-4876-9B99-7382B9A56D05}" name="TEST CASE ID" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{91B53198-5D1D-4488-AE13-BD7BDBF985C6}" name="TEST MODULE" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{C76204B1-4DBA-4279-AC5F-17173E9BFAE9}" name="TEST CASE SCENARIO" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{260BA782-8E33-473F-B547-7D03E1D0AEBA}" name="TEST CASE" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{765A51C0-A05E-4386-848D-E0FA301D9DB6}" name="PRE-CONDITION" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{FFC4DEB2-93EA-4AC4-97AC-50207431761C}" name="TEST STEPS" dataDxfId="67"/>
-    <tableColumn id="13" xr3:uid="{B3B38462-B4E8-4740-A145-E8888A2B69AA}" name="TEST DATE" dataDxfId="66"/>
-    <tableColumn id="7" xr3:uid="{86F842F8-C547-4C42-8C49-4CC8BA5F99B8}" name="TEST DATA" dataDxfId="65"/>
-    <tableColumn id="8" xr3:uid="{73BA7CDA-FD6A-4A79-966D-7E522D40E39A}" name="EXPECTED RESULT" dataDxfId="64"/>
-    <tableColumn id="9" xr3:uid="{0256B679-020D-472F-8363-0272EF10023F}" name="ACTTUAL RESULT" dataDxfId="63"/>
-    <tableColumn id="10" xr3:uid="{22950260-DDD6-44F4-94AF-051D113EEC57}" name="STATUS" dataDxfId="62"/>
-    <tableColumn id="11" xr3:uid="{8F220D65-B730-462C-9569-A73C01B5BD43}" name="Automate Test" dataDxfId="61"/>
-    <tableColumn id="12" xr3:uid="{C0E1154D-2A5C-485F-B063-63CCF8EBBA1D}" name="STATUS2" dataDxfId="60"/>
+    <tableColumn id="1" name="TEST CASE ID" dataDxfId="72"/>
+    <tableColumn id="2" name="TEST MODULE" dataDxfId="71"/>
+    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="70"/>
+    <tableColumn id="4" name="TEST CASE" dataDxfId="69"/>
+    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="68"/>
+    <tableColumn id="6" name="TEST STEPS" dataDxfId="67"/>
+    <tableColumn id="13" name="TEST DATE" dataDxfId="66"/>
+    <tableColumn id="7" name="TEST DATA" dataDxfId="65"/>
+    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="64"/>
+    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="63"/>
+    <tableColumn id="10" name="STATUS" dataDxfId="62"/>
+    <tableColumn id="11" name="Automate Test" dataDxfId="61"/>
+    <tableColumn id="12" name="STATUS2" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4FB980C6-3B05-4A5B-AEBE-713D936842C7}" name="Table135" displayName="Table135" ref="A8:M20" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
-  <autoFilter ref="A8:M20" xr:uid="{4FB980C6-3B05-4A5B-AEBE-713D936842C7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A8:M20" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+  <autoFilter ref="A8:M20"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6874EBC9-9793-4E74-9996-3754309E9A87}" name="TEST CASE ID" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{D9038A2B-1BEE-4892-8E44-B199F30269D4}" name="TEST MODULE" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{BD663D9F-2D61-4B34-B099-C62323C82AFF}" name="TEST CASE SCENARIO" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{7036D69E-10F3-4388-B3D5-8DED3E8FDCD6}" name="TEST CASE" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{621824A7-F6E2-4AA5-907F-03D69163A0DD}" name="PRE-CONDITION" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{341892DF-F2A6-4BED-8475-B7644ADE4089}" name="TEST STEPS" dataDxfId="52"/>
-    <tableColumn id="13" xr3:uid="{89B2F16F-17A2-45A0-82E7-FF7570629150}" name="TEST DATE" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{961BAE16-5564-4DDB-B9DB-13ABE0534CDB}" name="TEST DATA" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{006F5BEF-4670-446D-8893-3E8E09B0565F}" name="EXPECTED RESULT" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{E151C7A6-51FD-423E-A3AB-9AAF3BF3EA13}" name="ACTTUAL RESULT" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{25AA886A-0403-4D11-922C-26C1C27B8E68}" name="STATUS" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{F046929E-59BA-4006-836B-8977457D22B7}" name="Automate Test" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{C4A90A33-37AA-4D22-89D7-023B89E8DB92}" name="STATUS2" dataDxfId="45"/>
+    <tableColumn id="1" name="TEST CASE ID" dataDxfId="57"/>
+    <tableColumn id="2" name="TEST MODULE" dataDxfId="56"/>
+    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="55"/>
+    <tableColumn id="4" name="TEST CASE" dataDxfId="54"/>
+    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="53"/>
+    <tableColumn id="6" name="TEST STEPS" dataDxfId="52"/>
+    <tableColumn id="13" name="TEST DATE" dataDxfId="51"/>
+    <tableColumn id="7" name="TEST DATA" dataDxfId="50"/>
+    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="49"/>
+    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="48"/>
+    <tableColumn id="10" name="STATUS" dataDxfId="47"/>
+    <tableColumn id="11" name="Automate Test" dataDxfId="46"/>
+    <tableColumn id="12" name="STATUS2" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7D0E1F6E-E77C-4133-9287-8186AF22F72C}" name="Table136" displayName="Table136" ref="A8:M22" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="A8:M22" xr:uid="{7D0E1F6E-E77C-4133-9287-8186AF22F72C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table136" displayName="Table136" ref="A8:M22" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+  <autoFilter ref="A8:M22"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6A447137-1521-4CAA-ACE0-A135B80E55E2}" name="TEST CASE ID" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{0410A3EE-69AD-4DB2-9E61-46F6A72AEF8E}" name="TEST MODULE" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{96DA53B6-4EE9-4759-8295-0162BAC65A63}" name="TEST CASE SCENARIO" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{A049B43B-4CAA-4C87-AF00-775E61F79A51}" name="TEST CASE" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{3F757939-090E-4905-86FF-A48656A02B66}" name="PRE-CONDITION" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{733B7E1C-0B95-4A38-9DE2-CB36422740C8}" name="TEST STEPS" dataDxfId="37"/>
-    <tableColumn id="13" xr3:uid="{2A3EA811-AA08-4EA4-B332-6555E124F8E3}" name="TEST DATE" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{FD4A8BAC-9E65-4271-8BFF-B8226E14C13C}" name="TEST DATA" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{F4080DE1-CC88-4D9A-B57E-CB7D8E3D7EDF}" name="EXPECTED RESULT" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{6ADA73D6-5C34-4C7F-8F21-491C70C1C988}" name="ACTTUAL RESULT" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{95E4AB0D-8677-4A70-B522-6E2A6D225EEC}" name="STATUS" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{192D98B6-B78E-495F-8C53-CDC8F96DE062}" name="Automate Test" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{FA8C70D0-9F07-413D-9430-4E50DFB3163D}" name="STATUS2" dataDxfId="30"/>
+    <tableColumn id="1" name="TEST CASE ID" dataDxfId="42"/>
+    <tableColumn id="2" name="TEST MODULE" dataDxfId="41"/>
+    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="40"/>
+    <tableColumn id="4" name="TEST CASE" dataDxfId="39"/>
+    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="38"/>
+    <tableColumn id="6" name="TEST STEPS" dataDxfId="37"/>
+    <tableColumn id="13" name="TEST DATE" dataDxfId="36"/>
+    <tableColumn id="7" name="TEST DATA" dataDxfId="35"/>
+    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="34"/>
+    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="33"/>
+    <tableColumn id="10" name="STATUS" dataDxfId="32"/>
+    <tableColumn id="11" name="Automate Test" dataDxfId="31"/>
+    <tableColumn id="12" name="STATUS2" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E6C8870B-AB5C-49D8-AE20-FAD51DEDF595}" name="Table137" displayName="Table137" ref="A8:M17" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A8:M17" xr:uid="{E6C8870B-AB5C-49D8-AE20-FAD51DEDF595}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A8:M17" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A8:M17"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{6F1CB1B3-43A4-4DA1-AC5D-A968E9BA688C}" name="TEST CASE ID" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{F2683CB2-E4B3-4A4D-9BD2-FD0502960681}" name="TEST MODULE" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{01D25FA2-F21E-4B0D-8D7F-05668C21F5EF}" name="TEST CASE SCENARIO" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{74CF76EF-2F12-4BB7-872D-280D4AD4E894}" name="TEST CASE" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{5B5E5A88-235E-4974-B5F1-8F364C68073C}" name="PRE-CONDITION" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{02B7CAFF-DC06-4146-838F-5647562CCA14}" name="TEST STEPS" dataDxfId="22"/>
-    <tableColumn id="13" xr3:uid="{17815251-20FD-4FF3-92EA-DE5863F1A101}" name="TEST DATE" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{5AA73272-74D4-4744-B29D-755857977CDF}" name="TEST DATA" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{B402E435-D524-4FD6-8CA3-0E61BC31B905}" name="EXPECTED RESULT" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{AE1755E7-F33E-478F-AD2D-41A509E1B11F}" name="ACTTUAL RESULT" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{B9560BBE-2842-4969-9D19-14B816D187A6}" name="STATUS" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{61E8B746-E602-467E-9B39-E269B3C74333}" name="Automate Test" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{B0F2A006-83AE-464F-8D4D-4ED5348663BD}" name="STATUS2" dataDxfId="15"/>
+    <tableColumn id="1" name="TEST CASE ID" dataDxfId="27"/>
+    <tableColumn id="2" name="TEST MODULE" dataDxfId="26"/>
+    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="25"/>
+    <tableColumn id="4" name="TEST CASE" dataDxfId="24"/>
+    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="23"/>
+    <tableColumn id="6" name="TEST STEPS" dataDxfId="22"/>
+    <tableColumn id="13" name="TEST DATE" dataDxfId="21"/>
+    <tableColumn id="7" name="TEST DATA" dataDxfId="20"/>
+    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="19"/>
+    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="18"/>
+    <tableColumn id="10" name="STATUS" dataDxfId="17"/>
+    <tableColumn id="11" name="Automate Test" dataDxfId="16"/>
+    <tableColumn id="12" name="STATUS2" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5C213848-4C55-4CE7-999F-F5D5A3E526C1}" name="Table1379" displayName="Table1379" ref="A8:M16" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A8:M16" xr:uid="{5C213848-4C55-4CE7-999F-F5D5A3E526C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1379" displayName="Table1379" ref="A8:M16" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A8:M16"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{9FED8838-5AD5-4F78-95CA-9BAA85F07880}" name="TEST CASE ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{5EA252B4-17D4-4E7F-84E2-AAB55BB8C1FC}" name="TEST MODULE" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{76824998-B658-4D81-B2B1-39D99DF81B69}" name="TEST CASE SCENARIO" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{7DC07503-C2B9-4457-909F-D74460D5544B}" name="TEST CASE" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{B3435BA9-E1BA-4030-91C9-42D8816D3EB0}" name="PRE-CONDITION" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{CD1A9447-1674-474B-9ED7-2CF4CBDFF095}" name="TEST STEPS" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{94FB1A2F-9735-4A8D-9F12-C5F07A3263B0}" name="TEST DATE" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{F3826F7A-E610-4BFC-9C7C-8AB97E73A87A}" name="TEST DATA" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{C218831E-5987-4276-8B3B-31733F2D4EF9}" name="EXPECTED RESULT" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{6C4A78A1-763A-4006-A643-27B0ED9A9AEF}" name="ACTTUAL RESULT" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{AE70CEE4-F391-4282-9E7B-303E3DDDFE74}" name="STATUS" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{B26378C7-E69E-4C93-A9FD-487AB058274C}" name="Automate Test" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{7B714445-3764-41EF-B801-B9B6A17FC2B5}" name="STATUS2" dataDxfId="0"/>
+    <tableColumn id="1" name="TEST CASE ID" dataDxfId="12"/>
+    <tableColumn id="2" name="TEST MODULE" dataDxfId="11"/>
+    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="10"/>
+    <tableColumn id="4" name="TEST CASE" dataDxfId="9"/>
+    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="8"/>
+    <tableColumn id="6" name="TEST STEPS" dataDxfId="7"/>
+    <tableColumn id="13" name="TEST DATE" dataDxfId="6"/>
+    <tableColumn id="7" name="TEST DATA" dataDxfId="5"/>
+    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="4"/>
+    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="3"/>
+    <tableColumn id="10" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="11" name="Automate Test" dataDxfId="1"/>
+    <tableColumn id="12" name="STATUS2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2033,27 +2022,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08003585-1156-40A3-9017-127DA80E7316}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -2069,7 +2058,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2077,7 +2066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2088,7 +2077,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2096,7 +2085,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2137,7 +2126,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
@@ -2161,7 +2150,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
@@ -2197,7 +2186,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
@@ -2229,7 +2218,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
@@ -2265,7 +2254,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="56" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
@@ -2301,7 +2290,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -2347,27 +2336,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D36F27-A3EF-4854-AAD6-60F9FB603EDB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2375,7 +2364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -2383,7 +2372,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2391,7 +2380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2402,7 +2391,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2410,7 +2399,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2451,7 +2440,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>36</v>
       </c>
@@ -2476,7 +2465,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="56" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
@@ -2510,7 +2499,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="84" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
@@ -2542,7 +2531,7 @@
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
@@ -2574,7 +2563,7 @@
       <c r="L12" s="11"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>40</v>
       </c>
@@ -2606,7 +2595,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>41</v>
       </c>
@@ -2638,9 +2627,11 @@
       <c r="L14" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="M14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="M14" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="168" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>43</v>
       </c>
@@ -2677,7 +2668,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="168" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>48</v>
       </c>
@@ -2714,9 +2705,11 @@
       <c r="L16" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="M16" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="168" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>49</v>
       </c>
@@ -2753,7 +2746,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>50</v>
       </c>
@@ -2790,9 +2783,11 @@
       <c r="L18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="M18" s="9"/>
-    </row>
-    <row r="19" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="M18" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="168" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>61</v>
       </c>
@@ -2827,9 +2822,11 @@
       <c r="L19" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="M19" s="9"/>
-    </row>
-    <row r="20" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="M19" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="98" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>184</v>
       </c>
@@ -2876,31 +2873,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14F2252-5B28-4212-89F4-1C55D5288903}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView topLeftCell="C10" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.58203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.4140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2908,7 +2905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -2916,7 +2913,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2924,7 +2921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2935,7 +2932,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2943,7 +2940,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2984,7 +2981,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>88</v>
       </c>
@@ -3019,7 +3016,7 @@
       <c r="L9" s="13"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>92</v>
       </c>
@@ -3056,7 +3053,7 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>93</v>
       </c>
@@ -3091,7 +3088,7 @@
       <c r="L11" s="13"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>94</v>
       </c>
@@ -3128,7 +3125,7 @@
       </c>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>95</v>
       </c>
@@ -3163,7 +3160,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>96</v>
       </c>
@@ -3198,7 +3195,7 @@
       <c r="L14" s="13"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>97</v>
       </c>
@@ -3233,7 +3230,7 @@
       <c r="L15" s="13"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>98</v>
       </c>
@@ -3268,7 +3265,7 @@
       <c r="L16" s="13"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="112" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>107</v>
       </c>
@@ -3307,7 +3304,7 @@
       </c>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="98" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>108</v>
       </c>
@@ -3344,7 +3341,7 @@
       <c r="L18" s="13"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="98" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>109</v>
       </c>
@@ -3383,7 +3380,7 @@
       </c>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="98" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>110</v>
       </c>
@@ -3420,7 +3417,7 @@
       <c r="L20" s="13"/>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="98" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>111</v>
       </c>
@@ -3459,7 +3456,7 @@
       </c>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="112" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>112</v>
       </c>
@@ -3506,27 +3503,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12ED4BB2-0286-4A63-88C4-ADF727339384}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView topLeftCell="C10" workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3534,7 +3531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -3542,7 +3539,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -3550,7 +3547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3561,7 +3558,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -3569,7 +3566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -3610,7 +3607,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="56" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>135</v>
       </c>
@@ -3636,7 +3633,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="112" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>145</v>
       </c>
@@ -3672,7 +3669,7 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>146</v>
       </c>
@@ -3708,7 +3705,7 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>148</v>
       </c>
@@ -3743,7 +3740,7 @@
       <c r="L12" s="13"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>155</v>
       </c>
@@ -3780,7 +3777,7 @@
       </c>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>158</v>
       </c>
@@ -3815,7 +3812,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>159</v>
       </c>
@@ -3850,7 +3847,7 @@
       <c r="L15" s="13"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="56" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>160</v>
       </c>
@@ -3885,7 +3882,7 @@
       <c r="L16" s="13"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>161</v>
       </c>
@@ -3930,27 +3927,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5065EF-7FC3-4B75-9B16-995B989897B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3958,7 +3955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -3966,7 +3963,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -3974,7 +3971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3985,7 +3982,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -3993,7 +3990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -4034,7 +4031,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="56" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>162</v>
       </c>
@@ -4060,7 +4057,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>169</v>
       </c>
@@ -4094,7 +4091,7 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>170</v>
       </c>
@@ -4130,7 +4127,7 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="28" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>171</v>
       </c>
@@ -4165,7 +4162,7 @@
       <c r="L12" s="13"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="70" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>172</v>
       </c>
@@ -4200,7 +4197,7 @@
       <c r="L13" s="13"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>173</v>
       </c>
@@ -4235,7 +4232,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>174</v>
       </c>
@@ -4270,7 +4267,7 @@
       <c r="L15" s="13"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="42" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>175</v>
       </c>

</xml_diff>

<commit_message>
[Update] Folder structures, gitignore, keywords
Updated Folder structure [change keywords and loator to POM]
Updated gitignore
Updated Keywords
</commit_message>
<xml_diff>
--- a/CURA_TCs.xlsx
+++ b/CURA_TCs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visans49\Desktop\BOSS_GIT\CURA\web-cura-robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\web-cura-robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18D3BFE-94F0-409A-93FE-D5DD92E330BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
@@ -23,21 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="192">
   <si>
     <t>Project Name:</t>
   </si>
@@ -178,7 +170,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -188,7 +180,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -198,7 +190,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -208,7 +200,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -223,7 +215,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -233,7 +225,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -243,7 +235,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -253,7 +245,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -268,7 +260,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -278,7 +270,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -288,7 +280,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -298,7 +290,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -313,7 +305,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -323,7 +315,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -333,7 +325,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -343,7 +335,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -387,7 +379,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -397,7 +389,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -408,7 +400,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -418,7 +410,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -433,7 +425,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -443,7 +435,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -454,7 +446,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -464,7 +456,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -665,7 +657,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -675,7 +667,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -712,7 +704,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -722,7 +714,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -741,7 +733,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -751,7 +743,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -770,7 +762,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -780,7 +772,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -799,7 +791,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -809,7 +801,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Tahoma"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1054,12 +1046,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1067,14 +1059,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1082,20 +1074,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1617,110 +1609,110 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:M14" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
-  <autoFilter ref="A8:M14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:M14" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+  <autoFilter ref="A8:M14" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="TEST CASE ID" dataDxfId="72"/>
-    <tableColumn id="2" name="TEST MODULE" dataDxfId="71"/>
-    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="70"/>
-    <tableColumn id="4" name="TEST CASE" dataDxfId="69"/>
-    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="68"/>
-    <tableColumn id="6" name="TEST STEPS" dataDxfId="67"/>
-    <tableColumn id="13" name="TEST DATE" dataDxfId="66"/>
-    <tableColumn id="7" name="TEST DATA" dataDxfId="65"/>
-    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="64"/>
-    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="63"/>
-    <tableColumn id="10" name="STATUS" dataDxfId="62"/>
-    <tableColumn id="11" name="Automate Test" dataDxfId="61"/>
-    <tableColumn id="12" name="STATUS2" dataDxfId="60"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TEST CASE ID" dataDxfId="72"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="TEST MODULE" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="TEST CASE SCENARIO" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="TEST CASE" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="PRE-CONDITION" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="TEST STEPS" dataDxfId="67"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="TEST DATE" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="TEST DATA" dataDxfId="65"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="EXPECTED RESULT" dataDxfId="64"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ACTTUAL RESULT" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="STATUS" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Automate Test" dataDxfId="61"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="STATUS2" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A8:M20" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
-  <autoFilter ref="A8:M20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table135" displayName="Table135" ref="A8:M20" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+  <autoFilter ref="A8:M20" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="TEST CASE ID" dataDxfId="57"/>
-    <tableColumn id="2" name="TEST MODULE" dataDxfId="56"/>
-    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="55"/>
-    <tableColumn id="4" name="TEST CASE" dataDxfId="54"/>
-    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="53"/>
-    <tableColumn id="6" name="TEST STEPS" dataDxfId="52"/>
-    <tableColumn id="13" name="TEST DATE" dataDxfId="51"/>
-    <tableColumn id="7" name="TEST DATA" dataDxfId="50"/>
-    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="49"/>
-    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="48"/>
-    <tableColumn id="10" name="STATUS" dataDxfId="47"/>
-    <tableColumn id="11" name="Automate Test" dataDxfId="46"/>
-    <tableColumn id="12" name="STATUS2" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TEST CASE ID" dataDxfId="57"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="TEST MODULE" dataDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="TEST CASE SCENARIO" dataDxfId="55"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="TEST CASE" dataDxfId="54"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="PRE-CONDITION" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="TEST STEPS" dataDxfId="52"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="TEST DATE" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="TEST DATA" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="EXPECTED RESULT" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="ACTTUAL RESULT" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="STATUS" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Automate Test" dataDxfId="46"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="STATUS2" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table136" displayName="Table136" ref="A8:M22" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="A8:M22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table136" displayName="Table136" ref="A8:M22" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+  <autoFilter ref="A8:M22" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="TEST CASE ID" dataDxfId="42"/>
-    <tableColumn id="2" name="TEST MODULE" dataDxfId="41"/>
-    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="40"/>
-    <tableColumn id="4" name="TEST CASE" dataDxfId="39"/>
-    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="38"/>
-    <tableColumn id="6" name="TEST STEPS" dataDxfId="37"/>
-    <tableColumn id="13" name="TEST DATE" dataDxfId="36"/>
-    <tableColumn id="7" name="TEST DATA" dataDxfId="35"/>
-    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="34"/>
-    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="33"/>
-    <tableColumn id="10" name="STATUS" dataDxfId="32"/>
-    <tableColumn id="11" name="Automate Test" dataDxfId="31"/>
-    <tableColumn id="12" name="STATUS2" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TEST CASE ID" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="TEST MODULE" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="TEST CASE SCENARIO" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="TEST CASE" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="PRE-CONDITION" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="TEST STEPS" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="TEST DATE" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="TEST DATA" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="EXPECTED RESULT" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="ACTTUAL RESULT" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="STATUS" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0200-00000B000000}" name="Automate Test" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="STATUS2" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table137" displayName="Table137" ref="A8:M17" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A8:M17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table137" displayName="Table137" ref="A8:M17" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A8:M17" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="TEST CASE ID" dataDxfId="27"/>
-    <tableColumn id="2" name="TEST MODULE" dataDxfId="26"/>
-    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="25"/>
-    <tableColumn id="4" name="TEST CASE" dataDxfId="24"/>
-    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="23"/>
-    <tableColumn id="6" name="TEST STEPS" dataDxfId="22"/>
-    <tableColumn id="13" name="TEST DATE" dataDxfId="21"/>
-    <tableColumn id="7" name="TEST DATA" dataDxfId="20"/>
-    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="19"/>
-    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="18"/>
-    <tableColumn id="10" name="STATUS" dataDxfId="17"/>
-    <tableColumn id="11" name="Automate Test" dataDxfId="16"/>
-    <tableColumn id="12" name="STATUS2" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TEST CASE ID" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="TEST MODULE" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="TEST CASE SCENARIO" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="TEST CASE" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="PRE-CONDITION" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="TEST STEPS" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0300-00000D000000}" name="TEST DATE" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="TEST DATA" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="EXPECTED RESULT" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="ACTTUAL RESULT" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0300-00000A000000}" name="STATUS" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0300-00000B000000}" name="Automate Test" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0300-00000C000000}" name="STATUS2" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1379" displayName="Table1379" ref="A8:M16" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A8:M16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table1379" displayName="Table1379" ref="A8:M16" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A8:M16" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="TEST CASE ID" dataDxfId="12"/>
-    <tableColumn id="2" name="TEST MODULE" dataDxfId="11"/>
-    <tableColumn id="3" name="TEST CASE SCENARIO" dataDxfId="10"/>
-    <tableColumn id="4" name="TEST CASE" dataDxfId="9"/>
-    <tableColumn id="5" name="PRE-CONDITION" dataDxfId="8"/>
-    <tableColumn id="6" name="TEST STEPS" dataDxfId="7"/>
-    <tableColumn id="13" name="TEST DATE" dataDxfId="6"/>
-    <tableColumn id="7" name="TEST DATA" dataDxfId="5"/>
-    <tableColumn id="8" name="EXPECTED RESULT" dataDxfId="4"/>
-    <tableColumn id="9" name="ACTTUAL RESULT" dataDxfId="3"/>
-    <tableColumn id="10" name="STATUS" dataDxfId="2"/>
-    <tableColumn id="11" name="Automate Test" dataDxfId="1"/>
-    <tableColumn id="12" name="STATUS2" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TEST CASE ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="TEST MODULE" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="TEST CASE SCENARIO" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="TEST CASE" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="PRE-CONDITION" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="TEST STEPS" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="TEST DATE" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="TEST DATA" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="EXPECTED RESULT" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="ACTTUAL RESULT" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="Automate Test" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="STATUS2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2022,27 +2014,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2050,7 +2042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -2058,7 +2050,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2066,7 +2058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2077,7 +2069,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2085,7 +2077,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2126,7 +2118,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="70" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
@@ -2150,7 +2142,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
@@ -2186,7 +2178,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
@@ -2218,7 +2210,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>33</v>
       </c>
@@ -2254,7 +2246,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="56" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>34</v>
       </c>
@@ -2290,7 +2282,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -2336,27 +2328,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView topLeftCell="B14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2364,7 +2356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -2372,7 +2364,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2380,7 +2372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2391,7 +2383,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2399,7 +2391,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2440,7 +2432,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="70" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>36</v>
       </c>
@@ -2465,7 +2457,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="56" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>37</v>
       </c>
@@ -2499,7 +2491,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" ht="84" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
@@ -2531,7 +2523,7 @@
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
@@ -2563,7 +2555,7 @@
       <c r="L12" s="11"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>40</v>
       </c>
@@ -2595,7 +2587,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:13" ht="70" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>41</v>
       </c>
@@ -2631,7 +2623,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="168" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>43</v>
       </c>
@@ -2668,7 +2660,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="168" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>48</v>
       </c>
@@ -2709,7 +2701,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="168" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>49</v>
       </c>
@@ -2746,7 +2738,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>50</v>
       </c>
@@ -2787,7 +2779,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="168" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="180" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>61</v>
       </c>
@@ -2826,7 +2818,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="98" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>184</v>
       </c>
@@ -2873,31 +2865,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.58203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.4140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.58203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2905,7 +2897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -2913,7 +2905,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2921,7 +2913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2932,7 +2924,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2940,7 +2932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -2981,7 +2973,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="70" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>88</v>
       </c>
@@ -3016,7 +3008,7 @@
       <c r="L9" s="13"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>92</v>
       </c>
@@ -3051,9 +3043,11 @@
       <c r="L10" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+      <c r="M10" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>93</v>
       </c>
@@ -3088,7 +3082,7 @@
       <c r="L11" s="13"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>94</v>
       </c>
@@ -3125,7 +3119,7 @@
       </c>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>95</v>
       </c>
@@ -3160,7 +3154,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>96</v>
       </c>
@@ -3195,7 +3189,7 @@
       <c r="L14" s="13"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>97</v>
       </c>
@@ -3230,7 +3224,7 @@
       <c r="L15" s="13"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>98</v>
       </c>
@@ -3265,7 +3259,7 @@
       <c r="L16" s="13"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" ht="112" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>107</v>
       </c>
@@ -3304,7 +3298,7 @@
       </c>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13" ht="98" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>108</v>
       </c>
@@ -3341,7 +3335,7 @@
       <c r="L18" s="13"/>
       <c r="M18" s="9"/>
     </row>
-    <row r="19" spans="1:13" ht="98" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>109</v>
       </c>
@@ -3380,7 +3374,7 @@
       </c>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:13" ht="98" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>110</v>
       </c>
@@ -3417,7 +3411,7 @@
       <c r="L20" s="13"/>
       <c r="M20" s="9"/>
     </row>
-    <row r="21" spans="1:13" ht="98" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>111</v>
       </c>
@@ -3456,7 +3450,7 @@
       </c>
       <c r="M21" s="9"/>
     </row>
-    <row r="22" spans="1:13" ht="112" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>112</v>
       </c>
@@ -3503,27 +3497,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3531,7 +3525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -3539,7 +3533,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -3547,7 +3541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3558,7 +3552,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -3566,7 +3560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -3607,7 +3601,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="56" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>135</v>
       </c>
@@ -3633,7 +3627,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="112" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>145</v>
       </c>
@@ -3669,7 +3663,7 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>146</v>
       </c>
@@ -3705,7 +3699,7 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>148</v>
       </c>
@@ -3740,7 +3734,7 @@
       <c r="L12" s="13"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="70" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>155</v>
       </c>
@@ -3777,7 +3771,7 @@
       </c>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>158</v>
       </c>
@@ -3812,7 +3806,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>159</v>
       </c>
@@ -3847,7 +3841,7 @@
       <c r="L15" s="13"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="56" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>160</v>
       </c>
@@ -3882,7 +3876,7 @@
       <c r="L16" s="13"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>161</v>
       </c>
@@ -3927,27 +3921,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3955,7 +3949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>179</v>
       </c>
@@ -3963,7 +3957,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -3971,7 +3965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -3982,7 +3976,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -3990,7 +3984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -4031,7 +4025,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="56" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>162</v>
       </c>
@@ -4057,7 +4051,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>169</v>
       </c>
@@ -4091,7 +4085,7 @@
       </c>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>170</v>
       </c>
@@ -4127,7 +4121,7 @@
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>171</v>
       </c>
@@ -4162,7 +4156,7 @@
       <c r="L12" s="13"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="1:13" ht="70" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>172</v>
       </c>
@@ -4197,7 +4191,7 @@
       <c r="L13" s="13"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>173</v>
       </c>
@@ -4232,7 +4226,7 @@
       <c r="L14" s="12"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>174</v>
       </c>
@@ -4267,7 +4261,7 @@
       <c r="L15" s="13"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" ht="42" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>175</v>
       </c>

</xml_diff>

<commit_message>
[Update] Change word case
- Change Variable Naming cases.
</commit_message>
<xml_diff>
--- a/CURA_TCs.xlsx
+++ b/CURA_TCs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\web-cura-robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18D3BFE-94F0-409A-93FE-D5DD92E330BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043368AA-B276-461A-93E5-E693DAA5E000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="1875" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="192">
   <si>
     <t>Project Name:</t>
   </si>
@@ -2868,8 +2868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView topLeftCell="F22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,7 +3117,9 @@
       <c r="L12" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="M12" s="9"/>
+      <c r="M12" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
@@ -3296,7 +3298,9 @@
       <c r="L17" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="M17" s="9"/>
+      <c r="M17" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="18" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
@@ -3372,7 +3376,9 @@
       <c r="L19" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="M19" s="9"/>
+      <c r="M19" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
@@ -3448,7 +3454,9 @@
       <c r="L21" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="M21" s="9"/>
+      <c r="M21" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="22" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
@@ -3500,8 +3508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3924,7 +3932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>

</xml_diff>